<commit_message>
adds primitive cost calculation
</commit_message>
<xml_diff>
--- a/Simulation/data/building.xlsx
+++ b/Simulation/data/building.xlsx
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Bauteil</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>net_storey_height</t>
+  </si>
+  <si>
+    <t>differential_cost</t>
+  </si>
+  <si>
+    <t>€/m²BGF</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,6 +559,17 @@
       </c>
       <c r="C5" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -566,7 +583,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G5" sqref="G5:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>